<commit_message>
Fixed if multiple of the same setting
</commit_message>
<xml_diff>
--- a/Generating_Flight_Mission_Cycle/Flight_Mission_Cycle.xlsx
+++ b/Generating_Flight_Mission_Cycle/Flight_Mission_Cycle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac.sharepoint.com/teams/SmallJointImplantTestingRig/Shared Documents/General/11 - Code/GDP_47/Generating Flight Mission Cycle/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac.sharepoint.com/teams/SmallJointImplantTestingRig/Shared Documents/General/11 - Code/GDP_47/Generating_Flight_Mission_Cycle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{A43B4F40-E765-43F1-9A8D-784BFEF81CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D7F9715-7ACE-47B8-BE12-94DE20AF7041}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{A43B4F40-E765-43F1-9A8D-784BFEF81CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AA53A0C-C91C-420C-9C77-00F8E3A3A054}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="16080" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
+    <workbookView xWindow="1650" yWindow="16080" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
   </bookViews>
   <sheets>
     <sheet name="How to use" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="18">
   <si>
     <t>Setting</t>
   </si>
@@ -459,10 +459,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A671B1A1-7FE6-4148-92D2-482FECAD7275}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,7 +483,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -492,6 +492,14 @@
       </c>
       <c r="B3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -563,7 +571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF68743-A6F3-431E-B235-0E24B6BB11CE}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Working force dependent on angle
</commit_message>
<xml_diff>
--- a/Generating_Flight_Mission_Cycle/Flight_Mission_Cycle.xlsx
+++ b/Generating_Flight_Mission_Cycle/Flight_Mission_Cycle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac.sharepoint.com/teams/SmallJointImplantTestingRig/Shared Documents/General/11 - Code/GDP_47/Generating_Flight_Mission_Cycle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{A43B4F40-E765-43F1-9A8D-784BFEF81CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AA53A0C-C91C-420C-9C77-00F8E3A3A054}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="13_ncr:1_{A43B4F40-E765-43F1-9A8D-784BFEF81CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AE5AE8F-E2ED-4D70-A365-9780633D8CDC}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="16080" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
+    <workbookView xWindow="1650" yWindow="16080" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
   </bookViews>
   <sheets>
     <sheet name="How to use" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="21">
   <si>
     <t>Setting</t>
   </si>
@@ -56,46 +56,55 @@
     <t>Duration</t>
   </si>
   <si>
+    <t>Max_RoM</t>
+  </si>
+  <si>
+    <t>Min_RoM</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>Force</t>
+  </si>
+  <si>
+    <t>No. of cycles</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>set_points</t>
+  </si>
+  <si>
+    <t>RoM</t>
+  </si>
+  <si>
+    <t>sinosoidal</t>
+  </si>
+  <si>
+    <t>triangle</t>
+  </si>
+  <si>
+    <t>angle _dependent</t>
+  </si>
+  <si>
+    <t>Light switch</t>
+  </si>
+  <si>
+    <t>angle_dependent</t>
+  </si>
+  <si>
     <t>Typing</t>
   </si>
   <si>
-    <t>Max_RoM</t>
-  </si>
-  <si>
-    <t>Min_RoM</t>
-  </si>
-  <si>
-    <t>Period</t>
-  </si>
-  <si>
-    <t>Force</t>
-  </si>
-  <si>
-    <t>No. of cycles</t>
-  </si>
-  <si>
-    <t>Parameter</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>set_points</t>
-  </si>
-  <si>
-    <t>RoM</t>
-  </si>
-  <si>
-    <t>sinosoidal</t>
-  </si>
-  <si>
-    <t>triangle</t>
-  </si>
-  <si>
-    <t>angle _dependent</t>
-  </si>
-  <si>
-    <t>Light switch</t>
+    <t>&lt;1</t>
+  </si>
+  <si>
+    <t>&gt;10</t>
   </si>
 </sst>
 </file>
@@ -461,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A671B1A1-7FE6-4148-92D2-482FECAD7275}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,20 +484,20 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -496,7 +505,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -524,21 +533,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -548,18 +557,18 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -569,181 +578,78 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF68743-A6F3-431E-B235-0E24B6BB11CE}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>30</v>
-      </c>
-      <c r="E3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>-20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66F4A08-766D-4199-A7AF-6FAC79FAE8C9}">
-  <dimension ref="A1:F7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
       </c>
       <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="E3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
         <v>10</v>
       </c>
-      <c r="F3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
-      </c>
-      <c r="C5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
       </c>
       <c r="C6">
         <v>-20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -751,88 +657,183 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66F4A08-766D-4199-A7AF-6FAC79FAE8C9}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F28E5F9-7560-4700-BC16-43CF6FD42907}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
         <v>0</v>
-      </c>
-      <c r="C2">
-        <v>50</v>
       </c>
       <c r="D2">
         <v>50</v>
       </c>
       <c r="E2">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F2">
         <v>30</v>
       </c>
       <c r="G2">
+        <v>30</v>
+      </c>
+      <c r="H2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>20</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>30</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>10</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>100</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C6">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>-60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
+      <c r="C7">
         <v>10</v>
       </c>
     </row>
@@ -861,7 +862,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -901,7 +902,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>50</v>
@@ -909,7 +910,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>-20</v>
@@ -917,7 +918,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -929,26 +930,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010027F16B06E6E01148813C7ACA97AA34EF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fa346ec97cd2b8cb95951b4135646f8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a58a784a-84fb-458e-a075-e295952a81e3" xmlns:ns3="685e9b33-d6f8-42eb-aee1-d32c251952d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cdd15de96697d00dd4eeb440d71a501f" ns2:_="" ns3:_="">
     <xsd:import namespace="a58a784a-84fb-458e-a075-e295952a81e3"/>
@@ -1183,26 +1164,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
-    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F12FEC0-8F9C-493A-8210-061C1FAC29C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1219,4 +1201,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
+    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Complete ramp up function
</commit_message>
<xml_diff>
--- a/Generating_Flight_Mission_Cycle/Flight_Mission_Cycle.xlsx
+++ b/Generating_Flight_Mission_Cycle/Flight_Mission_Cycle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac.sharepoint.com/teams/SmallJointImplantTestingRig/Shared Documents/General/11 - Code/GDP_47/Generating_Flight_Mission_Cycle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="13_ncr:1_{A43B4F40-E765-43F1-9A8D-784BFEF81CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6AE5AE8F-E2ED-4D70-A365-9780633D8CDC}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{A43B4F40-E765-43F1-9A8D-784BFEF81CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE992F22-3114-4BFE-A201-6B07B0A66EAE}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="16080" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
   </bookViews>
   <sheets>
     <sheet name="How to use" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="21">
   <si>
     <t>Setting</t>
   </si>
@@ -468,10 +468,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A671B1A1-7FE6-4148-92D2-482FECAD7275}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,15 +500,7 @@
         <v>16</v>
       </c>
       <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -580,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF68743-A6F3-431E-B235-0E24B6BB11CE}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,7 +617,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -633,7 +625,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -641,7 +633,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>-20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -649,7 +641,7 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -661,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66F4A08-766D-4199-A7AF-6FAC79FAE8C9}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,7 +714,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>-20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -930,6 +922,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010027F16B06E6E01148813C7ACA97AA34EF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fa346ec97cd2b8cb95951b4135646f8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a58a784a-84fb-458e-a075-e295952a81e3" xmlns:ns3="685e9b33-d6f8-42eb-aee1-d32c251952d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cdd15de96697d00dd4eeb440d71a501f" ns2:_="" ns3:_="">
     <xsd:import namespace="a58a784a-84fb-458e-a075-e295952a81e3"/>
@@ -1164,27 +1176,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
+    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F12FEC0-8F9C-493A-8210-061C1FAC29C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1201,23 +1212,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
-    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Created function to write output file
</commit_message>
<xml_diff>
--- a/Generating_Flight_Mission_Cycle/Flight_Mission_Cycle.xlsx
+++ b/Generating_Flight_Mission_Cycle/Flight_Mission_Cycle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac.sharepoint.com/teams/SmallJointImplantTestingRig/Shared Documents/General/11 - Code/GDP_47/Generating_Flight_Mission_Cycle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{A43B4F40-E765-43F1-9A8D-784BFEF81CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE992F22-3114-4BFE-A201-6B07B0A66EAE}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="13_ncr:1_{A43B4F40-E765-43F1-9A8D-784BFEF81CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6749A02-133C-4513-AFDF-FDD43F77BADE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
+    <workbookView xWindow="1650" yWindow="16080" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
   </bookViews>
   <sheets>
     <sheet name="How to use" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="21">
   <si>
     <t>Setting</t>
   </si>
@@ -468,10 +468,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A671B1A1-7FE6-4148-92D2-482FECAD7275}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,6 +501,14 @@
       </c>
       <c r="B3">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -572,7 +580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF68743-A6F3-431E-B235-0E24B6BB11CE}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -922,26 +930,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010027F16B06E6E01148813C7ACA97AA34EF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fa346ec97cd2b8cb95951b4135646f8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a58a784a-84fb-458e-a075-e295952a81e3" xmlns:ns3="685e9b33-d6f8-42eb-aee1-d32c251952d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cdd15de96697d00dd4eeb440d71a501f" ns2:_="" ns3:_="">
     <xsd:import namespace="a58a784a-84fb-458e-a075-e295952a81e3"/>
@@ -1176,26 +1164,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
-    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F12FEC0-8F9C-493A-8210-061C1FAC29C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1212,4 +1201,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
+    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Now reads previous flight mission cycle and adds to new flight mission cycle
</commit_message>
<xml_diff>
--- a/Generating_Flight_Mission_Cycle/Flight_Mission_Cycle.xlsx
+++ b/Generating_Flight_Mission_Cycle/Flight_Mission_Cycle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac.sharepoint.com/teams/SmallJointImplantTestingRig/Shared Documents/General/11 - Code/GDP_47/Generating_Flight_Mission_Cycle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="13_ncr:1_{A43B4F40-E765-43F1-9A8D-784BFEF81CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6749A02-133C-4513-AFDF-FDD43F77BADE}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{2C28364A-564E-410B-97FD-7EAA9775DC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D702E11-0E69-40C2-A78F-93E961F09A7B}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="16080" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
   </bookViews>
   <sheets>
     <sheet name="How to use" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
   <si>
     <t>Setting</t>
   </si>
@@ -92,19 +92,22 @@
     <t>angle _dependent</t>
   </si>
   <si>
+    <t>angle_dependent</t>
+  </si>
+  <si>
+    <t>&lt;1</t>
+  </si>
+  <si>
+    <t>&gt;10</t>
+  </si>
+  <si>
+    <t>Typing</t>
+  </si>
+  <si>
     <t>Light switch</t>
   </si>
   <si>
-    <t>angle_dependent</t>
-  </si>
-  <si>
-    <t>Typing</t>
-  </si>
-  <si>
-    <t>&lt;1</t>
-  </si>
-  <si>
-    <t>&gt;10</t>
+    <t>Read_output</t>
   </si>
 </sst>
 </file>
@@ -471,12 +474,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -489,7 +493,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -497,18 +501,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -521,7 +522,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +582,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,10 +604,10 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
       </c>
       <c r="D2">
         <v>20</v>
@@ -625,7 +626,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -633,7 +634,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -641,7 +642,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -662,7 +663,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K13" sqref="K13:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,10 +685,10 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>30</v>
@@ -722,7 +723,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -930,6 +931,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010027F16B06E6E01148813C7ACA97AA34EF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fa346ec97cd2b8cb95951b4135646f8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a58a784a-84fb-458e-a075-e295952a81e3" xmlns:ns3="685e9b33-d6f8-42eb-aee1-d32c251952d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cdd15de96697d00dd4eeb440d71a501f" ns2:_="" ns3:_="">
     <xsd:import namespace="a58a784a-84fb-458e-a075-e295952a81e3"/>
@@ -1164,27 +1185,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
+    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F12FEC0-8F9C-493A-8210-061C1FAC29C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1201,23 +1221,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
-    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Created functions for reading mission cycle
</commit_message>
<xml_diff>
--- a/Generating_Flight_Mission_Cycle/Flight_Mission_Cycle.xlsx
+++ b/Generating_Flight_Mission_Cycle/Flight_Mission_Cycle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac.sharepoint.com/teams/SmallJointImplantTestingRig/Shared Documents/General/11 - Code/GDP_47/Generating_Flight_Mission_Cycle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{2C28364A-564E-410B-97FD-7EAA9775DC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67FD5DEA-21B7-4855-9B29-AB6CC23493A2}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{2C28364A-564E-410B-97FD-7EAA9775DC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1DF4BFB-539E-4DC4-AC7E-BBBF58C37ACB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
   <si>
     <t>Setting</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Light switch</t>
+  </si>
+  <si>
+    <t>Read_output</t>
   </si>
 </sst>
 </file>
@@ -468,10 +471,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A671B1A1-7FE6-4148-92D2-482FECAD7275}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,6 +505,11 @@
       </c>
       <c r="B3">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -923,6 +931,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010027F16B06E6E01148813C7ACA97AA34EF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fa346ec97cd2b8cb95951b4135646f8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a58a784a-84fb-458e-a075-e295952a81e3" xmlns:ns3="685e9b33-d6f8-42eb-aee1-d32c251952d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cdd15de96697d00dd4eeb440d71a501f" ns2:_="" ns3:_="">
     <xsd:import namespace="a58a784a-84fb-458e-a075-e295952a81e3"/>
@@ -1157,27 +1185,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
+    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F12FEC0-8F9C-493A-8210-061C1FAC29C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1194,23 +1221,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
-    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates C++ file with arduino functions
</commit_message>
<xml_diff>
--- a/Generating_Flight_Mission_Cycle/Flight_Mission_Cycle.xlsx
+++ b/Generating_Flight_Mission_Cycle/Flight_Mission_Cycle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac.sharepoint.com/teams/SmallJointImplantTestingRig/Shared Documents/General/11 - Code/GDP_47/Generating_Flight_Mission_Cycle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{2C28364A-564E-410B-97FD-7EAA9775DC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1DF4BFB-539E-4DC4-AC7E-BBBF58C37ACB}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{355AF9C3-9208-4457-9C0B-E652CDD3756D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9187C0E1-B7F4-40A5-92BF-2C182DFE55B5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="20">
   <si>
     <t>Setting</t>
   </si>
@@ -95,19 +95,13 @@
     <t>angle_dependent</t>
   </si>
   <si>
-    <t>&lt;1</t>
-  </si>
-  <si>
-    <t>&gt;10</t>
-  </si>
-  <si>
     <t>Typing</t>
   </si>
   <si>
-    <t>Light switch</t>
-  </si>
-  <si>
-    <t>Read_output</t>
+    <t>&gt;15</t>
+  </si>
+  <si>
+    <t>&lt;3</t>
   </si>
 </sst>
 </file>
@@ -471,10 +465,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A671B1A1-7FE6-4148-92D2-482FECAD7275}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,23 +487,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -582,7 +571,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +596,7 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>20</v>
@@ -663,7 +652,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13:L13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,7 +733,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,19 +780,19 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
         <v>10</v>
       </c>
-      <c r="G3">
-        <v>100</v>
-      </c>
       <c r="H3">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -940,17 +929,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010027F16B06E6E01148813C7ACA97AA34EF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fa346ec97cd2b8cb95951b4135646f8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a58a784a-84fb-458e-a075-e295952a81e3" xmlns:ns3="685e9b33-d6f8-42eb-aee1-d32c251952d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cdd15de96697d00dd4eeb440d71a501f" ns2:_="" ns3:_="">
     <xsd:import namespace="a58a784a-84fb-458e-a075-e295952a81e3"/>
@@ -1185,6 +1163,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
   <ds:schemaRefs>
@@ -1194,17 +1183,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
-    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F12FEC0-8F9C-493A-8210-061C1FAC29C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1221,4 +1199,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
+    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>